<commit_message>
plain rag output commit
</commit_message>
<xml_diff>
--- a/results/comparison_CoTPlainLLM/CoTPlainLLM_consolidated.xlsx
+++ b/results/comparison_CoTPlainLLM/CoTPlainLLM_consolidated.xlsx
@@ -545,19 +545,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.07407407217121062</v>
+        <v>0.141666663517014</v>
       </c>
       <c r="D2" t="n">
-        <v>7.140827185224432e-84</v>
+        <v>0.0005473171512287499</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5663584470748901</v>
+        <v>0.5791069269180298</v>
       </c>
       <c r="F2" t="n">
-        <v>18.14295977011494</v>
+        <v>35.22681451612902</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1911069063386944</v>
+        <v>0.2781456953642384</v>
       </c>
       <c r="H2" t="n">
         <v>0.6</v>
@@ -575,13 +575,13 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>4.782039642333984</v>
+        <v>4.134233713150024</v>
       </c>
       <c r="N2" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O2" t="n">
-        <v>6.8</v>
+        <v>3.7</v>
       </c>
       <c r="P2" t="n">
         <v>1</v>
@@ -593,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>4.782037496566772</v>
+        <v>4.13422966003418</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -609,19 +609,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.08333333146701394</v>
+        <v>0.07407407190976992</v>
       </c>
       <c r="D3" t="n">
-        <v>1.832655440606112e-155</v>
+        <v>7.454914944566463e-232</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4493230879306793</v>
+        <v>0.4374878406524658</v>
       </c>
       <c r="F3" t="n">
-        <v>48.07467350746271</v>
+        <v>14.39170454545456</v>
       </c>
       <c r="G3" t="n">
-        <v>4.715596330275229</v>
+        <v>4.238532110091743</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -639,13 +639,13 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>6.088991165161133</v>
+        <v>5.136576414108276</v>
       </c>
       <c r="N3" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O3" t="n">
-        <v>11</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="P3" t="n">
         <v>1</v>
@@ -657,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>6.088988065719604</v>
+        <v>5.136573791503906</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -673,22 +673,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.2352941134948097</v>
+        <v>0.109289614970886</v>
       </c>
       <c r="D4" t="n">
-        <v>5.51070408624463e-80</v>
+        <v>4.398437695781896e-157</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6009904742240906</v>
+        <v>0.6200515627861023</v>
       </c>
       <c r="F4" t="n">
-        <v>45.92624661246614</v>
+        <v>31.91045454545457</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4027777777777778</v>
+        <v>0.2254273504273504</v>
       </c>
       <c r="H4" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -703,13 +703,13 @@
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>3.738694906234741</v>
+        <v>5.039453983306885</v>
       </c>
       <c r="N4" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O4" t="n">
-        <v>9.199999999999999</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="P4" t="n">
         <v>1</v>
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>3.73869252204895</v>
+        <v>5.039451599121094</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -737,22 +737,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.08196721114653323</v>
+        <v>0.1162790670942252</v>
       </c>
       <c r="D5" t="n">
-        <v>2.098194796476083e-161</v>
+        <v>6.825887552000587e-159</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6145520210266113</v>
+        <v>0.6259207129478455</v>
       </c>
       <c r="F5" t="n">
-        <v>40.5779301075269</v>
+        <v>33.8339030612245</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1833060556464812</v>
+        <v>0.2266775777414075</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -767,13 +767,13 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>4.869560241699219</v>
+        <v>4.273945808410645</v>
       </c>
       <c r="N5" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O5" t="n">
-        <v>12.8</v>
+        <v>13</v>
       </c>
       <c r="P5" t="n">
         <v>1</v>
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>4.86955738067627</v>
+        <v>4.273943424224854</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -801,22 +801,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1348314581795228</v>
+        <v>0.02469135686633141</v>
       </c>
       <c r="D6" t="n">
-        <v>4.546890554684087e-235</v>
+        <v>5.096246152817909e-243</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5820237994194031</v>
+        <v>0.513387143611908</v>
       </c>
       <c r="F6" t="n">
-        <v>16.23333333333338</v>
+        <v>18.77909090909094</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2574712643678161</v>
+        <v>0.1459770114942529</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.5</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -831,13 +831,13 @@
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>4.084644317626953</v>
+        <v>4.349722146987915</v>
       </c>
       <c r="N6" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O6" t="n">
-        <v>9.300000000000001</v>
+        <v>9.4</v>
       </c>
       <c r="P6" t="n">
         <v>1</v>
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>4.084641456604004</v>
+        <v>4.349719762802124</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
@@ -865,25 +865,25 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.2624999964277833</v>
+        <v>0.2339743556201204</v>
       </c>
       <c r="D7" t="n">
-        <v>0.004012838286248903</v>
+        <v>0.002332389238732543</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6769643425941467</v>
+        <v>0.6736142635345459</v>
       </c>
       <c r="F7" t="n">
-        <v>38.06813718140933</v>
+        <v>30.7474083354214</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3002618562700029</v>
+        <v>0.2589467558917661</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -895,13 +895,13 @@
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>10.0699143409729</v>
+        <v>9.195940494537354</v>
       </c>
       <c r="N7" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O7" t="n">
-        <v>10.8</v>
+        <v>11</v>
       </c>
       <c r="P7" t="n">
         <v>1</v>
@@ -913,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>10.06991195678711</v>
+        <v>9.195937871932983</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -929,22 +929,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.07462686313210076</v>
+        <v>0.2880886380055402</v>
       </c>
       <c r="D8" t="n">
-        <v>2.825303885455152e-159</v>
+        <v>0.04588090562933512</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5373494029045105</v>
+        <v>0.6340779662132263</v>
       </c>
       <c r="F8" t="n">
-        <v>39.33000000000001</v>
+        <v>54.31765362698292</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1805555555555556</v>
+        <v>0.5493055555555556</v>
       </c>
       <c r="H8" t="n">
-        <v>0.05</v>
+        <v>0.35</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
@@ -959,13 +959,13 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>6.484943866729736</v>
+        <v>8.197777986526489</v>
       </c>
       <c r="N8" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O8" t="n">
-        <v>9.9</v>
+        <v>11.2</v>
       </c>
       <c r="P8" t="n">
         <v>1</v>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>6.484940767288208</v>
+        <v>8.197775602340698</v>
       </c>
       <c r="T8" t="n">
         <v>0</v>
@@ -993,22 +993,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.2222222190290664</v>
+        <v>0.11428571235999</v>
       </c>
       <c r="D9" t="n">
-        <v>0.003608591579733655</v>
+        <v>4.00532761681085e-162</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5966229438781738</v>
+        <v>0.6327927112579346</v>
       </c>
       <c r="F9" t="n">
-        <v>53.78447368421055</v>
+        <v>55.13486486486485</v>
       </c>
       <c r="G9" t="n">
-        <v>0.261297798377752</v>
+        <v>0.1367323290845887</v>
       </c>
       <c r="H9" t="n">
-        <v>0.375</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
@@ -1023,13 +1023,13 @@
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>7.40520167350769</v>
+        <v>7.060674428939819</v>
       </c>
       <c r="N9" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O9" t="n">
-        <v>10.6</v>
+        <v>9.1</v>
       </c>
       <c r="P9" t="n">
         <v>1</v>
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>7.405199289321899</v>
+        <v>7.060672044754028</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -1057,28 +1057,28 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0890410929191688</v>
+        <v>0.2812499962189453</v>
       </c>
       <c r="D10" t="n">
-        <v>0.000298269877512904</v>
+        <v>0.02424405070197356</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5640645027160645</v>
+        <v>0.627058744430542</v>
       </c>
       <c r="F10" t="n">
-        <v>4.827115384615411</v>
+        <v>52.10689917127073</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2473544973544974</v>
+        <v>0.3485449735449735</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1875</v>
+        <v>0.3125</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" t="n">
         <v>0.5</v>
@@ -1087,13 +1087,13 @@
         <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>9.957436561584473</v>
+        <v>6.115735530853271</v>
       </c>
       <c r="N10" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O10" t="n">
-        <v>10.9</v>
+        <v>12</v>
       </c>
       <c r="P10" t="n">
         <v>1</v>
@@ -1105,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>9.957433938980103</v>
+        <v>6.11573314666748</v>
       </c>
       <c r="T10" t="n">
         <v>0</v>
@@ -1121,19 +1121,19 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.0645161278815817</v>
+        <v>0.09374999835175783</v>
       </c>
       <c r="D11" t="n">
-        <v>1.57699300764286e-170</v>
+        <v>4.021168597696674e-164</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6301330924034119</v>
+        <v>0.638729989528656</v>
       </c>
       <c r="F11" t="n">
-        <v>64.94642105263159</v>
+        <v>47.20670454545456</v>
       </c>
       <c r="G11" t="n">
-        <v>0.09130672498633133</v>
+        <v>0.1153635866593767</v>
       </c>
       <c r="H11" t="n">
         <v>0.05555555555555555</v>
@@ -1151,13 +1151,13 @@
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>7.426047801971436</v>
+        <v>6.209541320800781</v>
       </c>
       <c r="N11" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O11" t="n">
-        <v>11.3</v>
+        <v>9.1</v>
       </c>
       <c r="P11" t="n">
         <v>1</v>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>7.426045179367065</v>
+        <v>6.209538698196411</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -1185,28 +1185,28 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.1305637954484059</v>
+        <v>0.1565217361085486</v>
       </c>
       <c r="D12" t="n">
-        <v>5.089221928114268e-05</v>
+        <v>0.0002541745212872696</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5930665135383606</v>
+        <v>0.621222972869873</v>
       </c>
       <c r="F12" t="n">
-        <v>27.40961538461539</v>
+        <v>24.04270161290324</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2369020501138952</v>
+        <v>0.2374715261958998</v>
       </c>
       <c r="H12" t="n">
-        <v>0.3888888888888889</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
         <v>0.5</v>
@@ -1215,13 +1215,13 @@
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>7.777541875839233</v>
+        <v>5.249120950698853</v>
       </c>
       <c r="N12" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O12" t="n">
-        <v>9.199999999999999</v>
+        <v>12.4</v>
       </c>
       <c r="P12" t="n">
         <v>1</v>
@@ -1233,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>7.777539968490601</v>
+        <v>5.249118566513062</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
@@ -1249,22 +1249,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.2762148300809126</v>
+        <v>0.05177993446905668</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01348948791655086</v>
+        <v>3.936845896757376e-172</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6302212476730347</v>
+        <v>0.4828194975852966</v>
       </c>
       <c r="F13" t="n">
-        <v>64.4534921524664</v>
+        <v>31.88333333333335</v>
       </c>
       <c r="G13" t="n">
-        <v>0.315410199556541</v>
+        <v>0.07705099778270511</v>
       </c>
       <c r="H13" t="n">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
@@ -1279,13 +1279,13 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>7.794389247894287</v>
+        <v>7.497222661972046</v>
       </c>
       <c r="N13" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O13" t="n">
-        <v>11.3</v>
+        <v>9</v>
       </c>
       <c r="P13" t="n">
         <v>1</v>
@@ -1297,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>7.794386386871338</v>
+        <v>7.497220277786255</v>
       </c>
       <c r="T13" t="n">
         <v>0</v>
@@ -1313,28 +1313,28 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.1763085367317048</v>
+        <v>0.02446482979734233</v>
       </c>
       <c r="D14" t="n">
-        <v>1.951521282527963e-80</v>
+        <v>2.015565332658881e-238</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6087909936904907</v>
+        <v>0.5507700443267822</v>
       </c>
       <c r="F14" t="n">
-        <v>59.76219774011301</v>
+        <v>-8.835000000000008</v>
       </c>
       <c r="G14" t="n">
-        <v>0.2344444444444445</v>
+        <v>0.1733333333333333</v>
       </c>
       <c r="H14" t="n">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
         <v>0.5</v>
@@ -1343,13 +1343,13 @@
         <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>7.932989358901978</v>
+        <v>13.61809158325195</v>
       </c>
       <c r="N14" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O14" t="n">
-        <v>11</v>
+        <v>10.9</v>
       </c>
       <c r="P14" t="n">
         <v>1</v>
@@ -1361,7 +1361,7 @@
         <v>0</v>
       </c>
       <c r="S14" t="n">
-        <v>7.932987213134766</v>
+        <v>13.61808967590332</v>
       </c>
       <c r="T14" t="n">
         <v>0</v>
@@ -1377,19 +1377,19 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.2236842060249309</v>
+        <v>0.1818181769111571</v>
       </c>
       <c r="D15" t="n">
-        <v>2.400973375710513e-155</v>
+        <v>2.896948262956944e-155</v>
       </c>
       <c r="E15" t="n">
-        <v>0.594032347202301</v>
+        <v>0.6043574810028076</v>
       </c>
       <c r="F15" t="n">
-        <v>49.01918739635158</v>
+        <v>49.0246153846154</v>
       </c>
       <c r="G15" t="n">
-        <v>0.6177062374245473</v>
+        <v>0.9054325955734407</v>
       </c>
       <c r="H15" t="n">
         <v>0.5</v>
@@ -1407,13 +1407,13 @@
         <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>4.35365629196167</v>
+        <v>5.396770000457764</v>
       </c>
       <c r="N15" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O15" t="n">
-        <v>9.6</v>
+        <v>11</v>
       </c>
       <c r="P15" t="n">
         <v>1</v>
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>4.353653430938721</v>
+        <v>5.396767377853394</v>
       </c>
       <c r="T15" t="n">
         <v>0</v>
@@ -1441,28 +1441,28 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.3540669809207665</v>
+        <v>0.183908042142291</v>
       </c>
       <c r="D16" t="n">
-        <v>1.24821259236603e-78</v>
+        <v>7.391975305139942e-156</v>
       </c>
       <c r="E16" t="n">
-        <v>0.6746441721916199</v>
+        <v>0.665554940700531</v>
       </c>
       <c r="F16" t="n">
-        <v>64.7267105263158</v>
+        <v>30.37537500000002</v>
       </c>
       <c r="G16" t="n">
-        <v>0.7161198288159771</v>
+        <v>0.4265335235378032</v>
       </c>
       <c r="H16" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="n">
         <v>0.5</v>
@@ -1471,13 +1471,13 @@
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>6.440952062606812</v>
+        <v>6.398717403411865</v>
       </c>
       <c r="N16" t="n">
-        <v>2079.53515625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O16" t="n">
-        <v>9.9</v>
+        <v>10</v>
       </c>
       <c r="P16" t="n">
         <v>1</v>
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="S16" t="n">
-        <v>6.440949440002441</v>
+        <v>6.398712635040283</v>
       </c>
       <c r="T16" t="n">
         <v>0</v>
@@ -1505,19 +1505,19 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.1390374291400956</v>
+        <v>0.3116883068308316</v>
       </c>
       <c r="D17" t="n">
-        <v>2.055386837335107e-232</v>
+        <v>0.03159281119052556</v>
       </c>
       <c r="E17" t="n">
-        <v>0.6169323921203613</v>
+        <v>0.6629244089126587</v>
       </c>
       <c r="F17" t="n">
-        <v>27.12392857142859</v>
+        <v>48.4701671511628</v>
       </c>
       <c r="G17" t="n">
-        <v>0.4018817204301075</v>
+        <v>0.7271505376344086</v>
       </c>
       <c r="H17" t="n">
         <v>0.1428571428571428</v>
@@ -1526,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="n">
         <v>0.5</v>
@@ -1535,13 +1535,13 @@
         <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>6.544068098068237</v>
+        <v>5.351824998855591</v>
       </c>
       <c r="N17" t="n">
-        <v>2079.54296875</v>
+        <v>2153.53125</v>
       </c>
       <c r="O17" t="n">
-        <v>10.9</v>
+        <v>11</v>
       </c>
       <c r="P17" t="n">
         <v>1</v>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>6.544065475463867</v>
+        <v>5.351821660995483</v>
       </c>
       <c r="T17" t="n">
         <v>0</v>
@@ -1569,22 +1569,22 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.2935420708975533</v>
+        <v>0.2651072089758292</v>
       </c>
       <c r="D18" t="n">
-        <v>0.009560226320964978</v>
+        <v>0.01108060554245823</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6350542902946472</v>
+        <v>0.6225570440292358</v>
       </c>
       <c r="F18" t="n">
-        <v>66.20192567567571</v>
+        <v>38.00722283609576</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2605140186915888</v>
+        <v>0.2698598130841122</v>
       </c>
       <c r="H18" t="n">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1599,13 +1599,13 @@
         <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>6.603177785873413</v>
+        <v>7.194129467010498</v>
       </c>
       <c r="N18" t="n">
-        <v>2079.54296875</v>
+        <v>2153.53125</v>
       </c>
       <c r="O18" t="n">
-        <v>11.7</v>
+        <v>10.9</v>
       </c>
       <c r="P18" t="n">
         <v>1</v>
@@ -1617,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>6.603175163269043</v>
+        <v>7.194126844406128</v>
       </c>
       <c r="T18" t="n">
         <v>0</v>
@@ -1633,28 +1633,28 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.1241379284126041</v>
+        <v>0.1858974325248603</v>
       </c>
       <c r="D19" t="n">
-        <v>3.969401530577779e-06</v>
+        <v>0.000648679953836082</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5873892307281494</v>
+        <v>0.6231503486633301</v>
       </c>
       <c r="F19" t="n">
-        <v>38.43663135593221</v>
+        <v>40.03207792207795</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1931443638760712</v>
+        <v>0.2986156888595913</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1176470588235294</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
         <v>0.5</v>
@@ -1663,13 +1663,13 @@
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>6.527792930603027</v>
+        <v>8.445894479751587</v>
       </c>
       <c r="N19" t="n">
-        <v>2079.54296875</v>
+        <v>2153.53125</v>
       </c>
       <c r="O19" t="n">
-        <v>9.1</v>
+        <v>9.5</v>
       </c>
       <c r="P19" t="n">
         <v>1</v>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>6.527791023254395</v>
+        <v>8.445892333984375</v>
       </c>
       <c r="T19" t="n">
         <v>0</v>
@@ -1697,28 +1697,28 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.2242990617738571</v>
+        <v>0.1228668914125966</v>
       </c>
       <c r="D20" t="n">
-        <v>0.008046940144253572</v>
+        <v>2.398491411925597e-157</v>
       </c>
       <c r="E20" t="n">
-        <v>0.6553922891616821</v>
+        <v>0.5950940251350403</v>
       </c>
       <c r="F20" t="n">
-        <v>39.6115534883721</v>
+        <v>17.42937500000002</v>
       </c>
       <c r="G20" t="n">
-        <v>0.3818310858765082</v>
+        <v>0.220014194464159</v>
       </c>
       <c r="H20" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
         <v>0.5</v>
@@ -1727,13 +1727,13 @@
         <v>0</v>
       </c>
       <c r="M20" t="n">
-        <v>5.925588846206665</v>
+        <v>6.768708229064941</v>
       </c>
       <c r="N20" t="n">
-        <v>2079.54296875</v>
+        <v>2153.53125</v>
       </c>
       <c r="O20" t="n">
-        <v>12.1</v>
+        <v>11.7</v>
       </c>
       <c r="P20" t="n">
         <v>1</v>
@@ -1745,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>5.925586700439453</v>
+        <v>6.76870584487915</v>
       </c>
       <c r="T20" t="n">
         <v>0</v>
@@ -1761,19 +1761,19 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.1464968123558766</v>
+        <v>0.125827812080172</v>
       </c>
       <c r="D21" t="n">
-        <v>2.781832879955916e-81</v>
+        <v>4.553262207947495e-159</v>
       </c>
       <c r="E21" t="n">
-        <v>0.5249164700508118</v>
+        <v>0.5015246868133545</v>
       </c>
       <c r="F21" t="n">
-        <v>69.71130120481931</v>
+        <v>61.47346774193551</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1790368271954674</v>
+        <v>0.1529745042492918</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1791,13 +1791,13 @@
         <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>4.783555746078491</v>
+        <v>5.438708066940308</v>
       </c>
       <c r="N21" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O21" t="n">
-        <v>9.1</v>
+        <v>8.9</v>
       </c>
       <c r="P21" t="n">
         <v>1</v>
@@ -1809,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="S21" t="n">
-        <v>4.783553838729858</v>
+        <v>5.438706636428833</v>
       </c>
       <c r="T21" t="n">
         <v>0</v>
@@ -1825,28 +1825,28 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.261904758245642</v>
+        <v>0.3005464438614172</v>
       </c>
       <c r="D22" t="n">
-        <v>0.006904345496705605</v>
+        <v>0.03483033707006006</v>
       </c>
       <c r="E22" t="n">
-        <v>0.6074649691581726</v>
+        <v>0.6286254525184631</v>
       </c>
       <c r="F22" t="n">
-        <v>33.15856725146202</v>
+        <v>52.00000000000003</v>
       </c>
       <c r="G22" t="n">
-        <v>0.3387878787878788</v>
+        <v>0.4436363636363637</v>
       </c>
       <c r="H22" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="I22" t="n">
         <v>1</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="n">
         <v>0.5</v>
@@ -1855,13 +1855,13 @@
         <v>0</v>
       </c>
       <c r="M22" t="n">
-        <v>6.279569864273071</v>
+        <v>9.660991191864014</v>
       </c>
       <c r="N22" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O22" t="n">
-        <v>11.9</v>
+        <v>10.8</v>
       </c>
       <c r="P22" t="n">
         <v>1</v>
@@ -1873,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="S22" t="n">
-        <v>6.279567956924438</v>
+        <v>9.660988807678223</v>
       </c>
       <c r="T22" t="n">
         <v>0</v>
@@ -1889,22 +1889,22 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.2660550423614385</v>
+        <v>0.3018867883056665</v>
       </c>
       <c r="D23" t="n">
-        <v>0.003735548393644041</v>
+        <v>0.0214579049673606</v>
       </c>
       <c r="E23" t="n">
-        <v>0.630036473274231</v>
+        <v>0.648881196975708</v>
       </c>
       <c r="F23" t="n">
-        <v>16.27247219413553</v>
+        <v>42.04635179153095</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2903077629765733</v>
+        <v>0.3867707854846119</v>
       </c>
       <c r="H23" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -1919,13 +1919,13 @@
         <v>0</v>
       </c>
       <c r="M23" t="n">
-        <v>8.391186237335205</v>
+        <v>11.58311986923218</v>
       </c>
       <c r="N23" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O23" t="n">
-        <v>9.199999999999999</v>
+        <v>10.5</v>
       </c>
       <c r="P23" t="n">
         <v>1</v>
@@ -1937,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="S23" t="n">
-        <v>8.391183614730835</v>
+        <v>11.58311820030212</v>
       </c>
       <c r="T23" t="n">
         <v>0</v>
@@ -1953,22 +1953,22 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.1550387565651103</v>
+        <v>0.2658959489618765</v>
       </c>
       <c r="D24" t="n">
-        <v>4.632648588475813e-157</v>
+        <v>3.164234907918165e-155</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5878866910934448</v>
+        <v>0.6610466241836548</v>
       </c>
       <c r="F24" t="n">
-        <v>24.22750000000002</v>
+        <v>48.87895801526719</v>
       </c>
       <c r="G24" t="n">
-        <v>0.3410138248847926</v>
+        <v>0.6697388632872504</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
         <v>1</v>
@@ -1983,13 +1983,13 @@
         <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>5.019073247909546</v>
+        <v>4.264206886291504</v>
       </c>
       <c r="N24" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O24" t="n">
-        <v>12.5</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="P24" t="n">
         <v>1</v>
@@ -2001,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="S24" t="n">
-        <v>5.019070625305176</v>
+        <v>4.264204502105713</v>
       </c>
       <c r="T24" t="n">
         <v>0</v>
@@ -2017,19 +2017,19 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.2543352555848843</v>
+        <v>0.2872928129886146</v>
       </c>
       <c r="D25" t="n">
-        <v>1.183171534458101e-155</v>
+        <v>5.311101064356547e-79</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6302258968353271</v>
+        <v>0.6510871648788452</v>
       </c>
       <c r="F25" t="n">
-        <v>30.4377272727273</v>
+        <v>26.72375000000002</v>
       </c>
       <c r="G25" t="n">
-        <v>0.5641025641025641</v>
+        <v>0.6410256410256411</v>
       </c>
       <c r="H25" t="n">
         <v>1</v>
@@ -2047,13 +2047,13 @@
         <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>4.732515096664429</v>
+        <v>5.25409984588623</v>
       </c>
       <c r="N25" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O25" t="n">
-        <v>9</v>
+        <v>11.9</v>
       </c>
       <c r="P25" t="n">
         <v>1</v>
@@ -2065,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="S25" t="n">
-        <v>4.732512474060059</v>
+        <v>5.25409722328186</v>
       </c>
       <c r="T25" t="n">
         <v>0</v>
@@ -2081,19 +2081,19 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.09836065229105093</v>
+        <v>0.09022555982814197</v>
       </c>
       <c r="D26" t="n">
-        <v>3.057476153418618e-157</v>
+        <v>1.317797909784937e-156</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5557619333267212</v>
+        <v>0.5752767324447632</v>
       </c>
       <c r="F26" t="n">
-        <v>22.22387096774196</v>
+        <v>16.82500000000002</v>
       </c>
       <c r="G26" t="n">
-        <v>0.3934142114384749</v>
+        <v>0.4610051993067591</v>
       </c>
       <c r="H26" t="n">
         <v>1</v>
@@ -2111,13 +2111,13 @@
         <v>0</v>
       </c>
       <c r="M26" t="n">
-        <v>5.664849042892456</v>
+        <v>4.754911184310913</v>
       </c>
       <c r="N26" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O26" t="n">
-        <v>12.2</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="P26" t="n">
         <v>1</v>
@@ -2129,7 +2129,7 @@
         <v>0</v>
       </c>
       <c r="S26" t="n">
-        <v>5.664847135543823</v>
+        <v>4.754908800125122</v>
       </c>
       <c r="T26" t="n">
         <v>0</v>
@@ -2145,19 +2145,19 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.2525252479252118</v>
+        <v>0.2587064630093315</v>
       </c>
       <c r="D27" t="n">
-        <v>5.486664596027297e-79</v>
+        <v>5.137564652725544e-79</v>
       </c>
       <c r="E27" t="n">
-        <v>0.6652215719223022</v>
+        <v>0.6802657246589661</v>
       </c>
       <c r="F27" t="n">
-        <v>63.63412361178177</v>
+        <v>39.22636363636366</v>
       </c>
       <c r="G27" t="n">
-        <v>0.5841313269493844</v>
+        <v>0.6210670314637483</v>
       </c>
       <c r="H27" t="n">
         <v>1</v>
@@ -2175,13 +2175,13 @@
         <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>4.553334951400757</v>
+        <v>6.266167402267456</v>
       </c>
       <c r="N27" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O27" t="n">
-        <v>9</v>
+        <v>11.7</v>
       </c>
       <c r="P27" t="n">
         <v>1</v>
@@ -2193,7 +2193,7 @@
         <v>0</v>
       </c>
       <c r="S27" t="n">
-        <v>4.553332328796387</v>
+        <v>6.266165733337402</v>
       </c>
       <c r="T27" t="n">
         <v>0</v>
@@ -2209,19 +2209,19 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.1818181772217202</v>
+        <v>0.1754385920084814</v>
       </c>
       <c r="D28" t="n">
-        <v>4.243949549563547e-79</v>
+        <v>7.098725688238602e-156</v>
       </c>
       <c r="E28" t="n">
-        <v>0.6359030604362488</v>
+        <v>0.5641580820083618</v>
       </c>
       <c r="F28" t="n">
-        <v>25.82339060710197</v>
+        <v>31.61011940298511</v>
       </c>
       <c r="G28" t="n">
-        <v>0.5984848484848485</v>
+        <v>0.5242424242424243</v>
       </c>
       <c r="H28" t="n">
         <v>1</v>
@@ -2239,10 +2239,10 @@
         <v>0</v>
       </c>
       <c r="M28" t="n">
-        <v>4.642242193222046</v>
+        <v>4.107651233673096</v>
       </c>
       <c r="N28" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O28" t="n">
         <v>9.1</v>
@@ -2257,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="S28" t="n">
-        <v>4.642239570617676</v>
+        <v>4.107649087905884</v>
       </c>
       <c r="T28" t="n">
         <v>0</v>
@@ -2273,19 +2273,19 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.2820512772887903</v>
+        <v>0.2302158230112314</v>
       </c>
       <c r="D29" t="n">
-        <v>7.823029185358786e-156</v>
+        <v>1.563731692241463e-79</v>
       </c>
       <c r="E29" t="n">
-        <v>0.5909065008163452</v>
+        <v>0.5910755395889282</v>
       </c>
       <c r="F29" t="n">
-        <v>61.53617647058823</v>
+        <v>52.93923076923079</v>
       </c>
       <c r="G29" t="n">
-        <v>0.6336805555555556</v>
+        <v>0.6197916666666666</v>
       </c>
       <c r="H29" t="n">
         <v>1</v>
@@ -2303,10 +2303,10 @@
         <v>0</v>
       </c>
       <c r="M29" t="n">
-        <v>5.937963247299194</v>
+        <v>5.678453207015991</v>
       </c>
       <c r="N29" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O29" t="n">
         <v>12.1</v>
@@ -2321,7 +2321,7 @@
         <v>0</v>
       </c>
       <c r="S29" t="n">
-        <v>5.937960624694824</v>
+        <v>5.678450584411621</v>
       </c>
       <c r="T29" t="n">
         <v>0</v>
@@ -2337,25 +2337,25 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.1052631542797785</v>
+        <v>0.0439560421736506</v>
       </c>
       <c r="D30" t="n">
-        <v>3.160834788426398e-155</v>
+        <v>5.448548490014436e-232</v>
       </c>
       <c r="E30" t="n">
-        <v>0.5090331435203552</v>
+        <v>0.4455536901950836</v>
       </c>
       <c r="F30" t="n">
-        <v>45.1304761904762</v>
+        <v>37.12436948297608</v>
       </c>
       <c r="G30" t="n">
-        <v>2.23</v>
+        <v>5.07</v>
       </c>
       <c r="H30" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
         <v>1</v>
@@ -2367,10 +2367,10 @@
         <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>4.176806211471558</v>
+        <v>4.734951496124268</v>
       </c>
       <c r="N30" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O30" t="n">
         <v>9.1</v>
@@ -2385,7 +2385,7 @@
         <v>0</v>
       </c>
       <c r="S30" t="n">
-        <v>4.176803350448608</v>
+        <v>4.734949111938477</v>
       </c>
       <c r="T30" t="n">
         <v>0</v>
@@ -2401,22 +2401,22 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.114285712044898</v>
+        <v>0.1052631558067867</v>
       </c>
       <c r="D31" t="n">
-        <v>7.079893191305051e-79</v>
+        <v>1.998443100417405e-155</v>
       </c>
       <c r="E31" t="n">
-        <v>0.449518233537674</v>
+        <v>0.4741330444812775</v>
       </c>
       <c r="F31" t="n">
-        <v>56.66341114457833</v>
+        <v>32.11718131868133</v>
       </c>
       <c r="G31" t="n">
-        <v>3.660194174757282</v>
+        <v>3.990291262135922</v>
       </c>
       <c r="H31" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I31" t="n">
         <v>1</v>
@@ -2431,13 +2431,13 @@
         <v>0</v>
       </c>
       <c r="M31" t="n">
-        <v>3.777897119522095</v>
+        <v>4.281505346298218</v>
       </c>
       <c r="N31" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O31" t="n">
-        <v>12.7</v>
+        <v>9.1</v>
       </c>
       <c r="P31" t="n">
         <v>1</v>
@@ -2449,7 +2449,7 @@
         <v>0</v>
       </c>
       <c r="S31" t="n">
-        <v>3.777894735336304</v>
+        <v>4.281502723693848</v>
       </c>
       <c r="T31" t="n">
         <v>0</v>
@@ -2465,22 +2465,22 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.09876543012345682</v>
+        <v>0.1159420267170763</v>
       </c>
       <c r="D32" t="n">
-        <v>5.849159097634654e-79</v>
+        <v>2.512453984152669e-155</v>
       </c>
       <c r="E32" t="n">
-        <v>0.4674080610275269</v>
+        <v>0.455717921257019</v>
       </c>
       <c r="F32" t="n">
-        <v>41.23505062305296</v>
+        <v>27.4778758169935</v>
       </c>
       <c r="G32" t="n">
-        <v>4.42</v>
+        <v>3.82</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" t="n">
         <v>1</v>
@@ -2495,13 +2495,13 @@
         <v>0</v>
       </c>
       <c r="M32" t="n">
-        <v>5.303272247314453</v>
+        <v>4.544331789016724</v>
       </c>
       <c r="N32" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O32" t="n">
-        <v>9.800000000000001</v>
+        <v>13</v>
       </c>
       <c r="P32" t="n">
         <v>1</v>
@@ -2513,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="S32" t="n">
-        <v>5.303269863128662</v>
+        <v>4.544329404830933</v>
       </c>
       <c r="T32" t="n">
         <v>0</v>
@@ -2529,19 +2529,19 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.3013698583890037</v>
+        <v>0.2739725981150311</v>
       </c>
       <c r="D33" t="n">
-        <v>0.02966575148178999</v>
+        <v>4.311555525306547e-155</v>
       </c>
       <c r="E33" t="n">
-        <v>0.6513624787330627</v>
+        <v>0.6466585993766785</v>
       </c>
       <c r="F33" t="n">
-        <v>70.65908895265426</v>
+        <v>66.22013808975836</v>
       </c>
       <c r="G33" t="n">
-        <v>1.479224376731302</v>
+        <v>1.556786703601108</v>
       </c>
       <c r="H33" t="n">
         <v>0.3333333333333333</v>
@@ -2559,13 +2559,13 @@
         <v>0</v>
       </c>
       <c r="M33" t="n">
-        <v>6.744629621505737</v>
+        <v>7.359601497650146</v>
       </c>
       <c r="N33" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O33" t="n">
-        <v>11.3</v>
+        <v>9</v>
       </c>
       <c r="P33" t="n">
         <v>1</v>
@@ -2577,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="S33" t="n">
-        <v>6.744626998901367</v>
+        <v>7.359598398208618</v>
       </c>
       <c r="T33" t="n">
         <v>0</v>
@@ -2593,25 +2593,25 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.2330097038439062</v>
+        <v>0.2735849007244571</v>
       </c>
       <c r="D34" t="n">
-        <v>1.158776659102439e-78</v>
+        <v>1.424107872119102e-78</v>
       </c>
       <c r="E34" t="n">
-        <v>0.6419915556907654</v>
+        <v>0.6349708437919617</v>
       </c>
       <c r="F34" t="n">
-        <v>53.76202898550727</v>
+        <v>42.27932608695653</v>
       </c>
       <c r="G34" t="n">
-        <v>0.8299418604651163</v>
+        <v>0.8241279069767442</v>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="n">
         <v>1</v>
@@ -2623,13 +2623,13 @@
         <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>6.231465816497803</v>
+        <v>5.367925405502319</v>
       </c>
       <c r="N34" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O34" t="n">
-        <v>9.300000000000001</v>
+        <v>12.3</v>
       </c>
       <c r="P34" t="n">
         <v>1</v>
@@ -2641,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="S34" t="n">
-        <v>6.231463193893433</v>
+        <v>5.367923259735107</v>
       </c>
       <c r="T34" t="n">
         <v>0</v>
@@ -2657,28 +2657,28 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.2007721972123254</v>
+        <v>0.2625482589883872</v>
       </c>
       <c r="D35" t="n">
-        <v>1.57997522977731e-79</v>
+        <v>0.01029378225573462</v>
       </c>
       <c r="E35" t="n">
-        <v>0.6333149671554565</v>
+        <v>0.6615652441978455</v>
       </c>
       <c r="F35" t="n">
-        <v>44.70807692307693</v>
+        <v>46.8856725146199</v>
       </c>
       <c r="G35" t="n">
-        <v>0.3283712784588441</v>
+        <v>0.3204903677758319</v>
       </c>
       <c r="H35" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" t="n">
         <v>0.5</v>
@@ -2687,13 +2687,13 @@
         <v>0</v>
       </c>
       <c r="M35" t="n">
-        <v>4.985752105712891</v>
+        <v>3.368766784667969</v>
       </c>
       <c r="N35" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O35" t="n">
-        <v>11.2</v>
+        <v>9.1</v>
       </c>
       <c r="P35" t="n">
         <v>1</v>
@@ -2705,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="S35" t="n">
-        <v>4.9857497215271</v>
+        <v>3.36876392364502</v>
       </c>
       <c r="T35" t="n">
         <v>0</v>
@@ -2721,22 +2721,22 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.1699346370660858</v>
+        <v>0.2681564201242159</v>
       </c>
       <c r="D36" t="n">
-        <v>1.795848077170038e-155</v>
+        <v>0.0502954152315403</v>
       </c>
       <c r="E36" t="n">
-        <v>0.5833650231361389</v>
+        <v>0.7335803508758545</v>
       </c>
       <c r="F36" t="n">
-        <v>-2.652424749163856</v>
+        <v>24.30150000000003</v>
       </c>
       <c r="G36" t="n">
-        <v>0.4247226624405705</v>
+        <v>0.5625990491283677</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" t="n">
         <v>1</v>
@@ -2751,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>6.771903991699219</v>
+        <v>4.266078233718872</v>
       </c>
       <c r="N36" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O36" t="n">
-        <v>10.2</v>
+        <v>11.5</v>
       </c>
       <c r="P36" t="n">
         <v>1</v>
@@ -2769,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="S36" t="n">
-        <v>6.771901845932007</v>
+        <v>4.266075611114502</v>
       </c>
       <c r="T36" t="n">
         <v>0</v>
@@ -2785,28 +2785,28 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.2631578904155125</v>
+        <v>0.2008032081714813</v>
       </c>
       <c r="D37" t="n">
-        <v>0.01043196607067424</v>
+        <v>4.733002179416841e-79</v>
       </c>
       <c r="E37" t="n">
-        <v>0.6496437191963196</v>
+        <v>0.6041285991668701</v>
       </c>
       <c r="F37" t="n">
-        <v>52.56112820512823</v>
+        <v>38.05287581699349</v>
       </c>
       <c r="G37" t="n">
-        <v>0.4644750795334041</v>
+        <v>0.6044538706256628</v>
       </c>
       <c r="H37" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" t="n">
         <v>0.5</v>
@@ -2815,13 +2815,13 @@
         <v>0</v>
       </c>
       <c r="M37" t="n">
-        <v>6.82994556427002</v>
+        <v>9.039860725402832</v>
       </c>
       <c r="N37" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O37" t="n">
-        <v>11.5</v>
+        <v>9.9</v>
       </c>
       <c r="P37" t="n">
         <v>1</v>
@@ -2833,7 +2833,7 @@
         <v>0</v>
       </c>
       <c r="S37" t="n">
-        <v>6.829943180084229</v>
+        <v>9.03985857963562</v>
       </c>
       <c r="T37" t="n">
         <v>0</v>
@@ -2849,22 +2849,22 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.1919191873482299</v>
+        <v>0.2660944156495791</v>
       </c>
       <c r="D38" t="n">
-        <v>1.71144046761146e-155</v>
+        <v>7.534217237408934e-79</v>
       </c>
       <c r="E38" t="n">
-        <v>0.58353590965271</v>
+        <v>0.6522415280342102</v>
       </c>
       <c r="F38" t="n">
-        <v>30.86950000000002</v>
+        <v>44.32163043478263</v>
       </c>
       <c r="G38" t="n">
-        <v>0.5588615782664942</v>
+        <v>0.8382923673997412</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" t="n">
         <v>1</v>
@@ -2879,13 +2879,13 @@
         <v>0</v>
       </c>
       <c r="M38" t="n">
-        <v>9.056885004043579</v>
+        <v>6.725923776626587</v>
       </c>
       <c r="N38" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O38" t="n">
-        <v>9.199999999999999</v>
+        <v>11.6</v>
       </c>
       <c r="P38" t="n">
         <v>1</v>
@@ -2897,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="S38" t="n">
-        <v>9.056882619857788</v>
+        <v>6.725921392440796</v>
       </c>
       <c r="T38" t="n">
         <v>0</v>
@@ -2913,22 +2913,22 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.1257861592579409</v>
+        <v>0.0350877186211142</v>
       </c>
       <c r="D39" t="n">
-        <v>1.616310286165201e-155</v>
+        <v>4.552054890405703e-238</v>
       </c>
       <c r="E39" t="n">
-        <v>0.6308585405349731</v>
+        <v>0.4263676106929779</v>
       </c>
       <c r="F39" t="n">
-        <v>43.52442571127506</v>
+        <v>31.54500000000002</v>
       </c>
       <c r="G39" t="n">
-        <v>0.5294985250737463</v>
+        <v>0.1061946902654867</v>
       </c>
       <c r="H39" t="n">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="I39" t="n">
         <v>1</v>
@@ -2943,13 +2943,13 @@
         <v>0</v>
       </c>
       <c r="M39" t="n">
-        <v>8.633267402648926</v>
+        <v>7.392796516418457</v>
       </c>
       <c r="N39" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O39" t="n">
-        <v>11.1</v>
+        <v>9.9</v>
       </c>
       <c r="P39" t="n">
         <v>1</v>
@@ -2961,7 +2961,7 @@
         <v>0</v>
       </c>
       <c r="S39" t="n">
-        <v>8.633265495300293</v>
+        <v>7.392794847488403</v>
       </c>
       <c r="T39" t="n">
         <v>0</v>
@@ -2977,22 +2977,22 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.2280701710541706</v>
+        <v>0.3139013410179172</v>
       </c>
       <c r="D40" t="n">
-        <v>1.751721339189862e-79</v>
+        <v>0.004596827558957366</v>
       </c>
       <c r="E40" t="n">
-        <v>0.6069880127906799</v>
+        <v>0.6013320684432983</v>
       </c>
       <c r="F40" t="n">
-        <v>49.83830636461707</v>
+        <v>62.40452380952382</v>
       </c>
       <c r="G40" t="n">
-        <v>0.461453744493392</v>
+        <v>0.3953744493392071</v>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="I40" t="n">
         <v>1</v>
@@ -3007,13 +3007,13 @@
         <v>0</v>
       </c>
       <c r="M40" t="n">
-        <v>4.620523452758789</v>
+        <v>4.250593185424805</v>
       </c>
       <c r="N40" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O40" t="n">
-        <v>12.3</v>
+        <v>12.1</v>
       </c>
       <c r="P40" t="n">
         <v>1</v>
@@ -3025,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="S40" t="n">
-        <v>4.620521068572998</v>
+        <v>4.250590801239014</v>
       </c>
       <c r="T40" t="n">
         <v>0</v>
@@ -3041,22 +3041,22 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.06382978544540018</v>
+        <v>0.2624671871566054</v>
       </c>
       <c r="D41" t="n">
-        <v>1.841754956399447e-162</v>
+        <v>0.010847854323355</v>
       </c>
       <c r="E41" t="n">
-        <v>0.6188222169876099</v>
+        <v>0.6584652066230774</v>
       </c>
       <c r="F41" t="n">
-        <v>33.125</v>
+        <v>59.81312834224602</v>
       </c>
       <c r="G41" t="n">
-        <v>0.1481481481481481</v>
+        <v>0.4430727023319616</v>
       </c>
       <c r="H41" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="I41" t="n">
         <v>1</v>
@@ -3071,13 +3071,13 @@
         <v>0</v>
       </c>
       <c r="M41" t="n">
-        <v>3.897192239761353</v>
+        <v>5.721935272216797</v>
       </c>
       <c r="N41" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O41" t="n">
-        <v>9.800000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="P41" t="n">
         <v>1</v>
@@ -3089,7 +3089,7 @@
         <v>0</v>
       </c>
       <c r="S41" t="n">
-        <v>3.897189617156982</v>
+        <v>5.721932172775269</v>
       </c>
       <c r="T41" t="n">
         <v>0</v>
@@ -3105,22 +3105,22 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.09411764516539796</v>
+        <v>0.1111111084839507</v>
       </c>
       <c r="D42" t="n">
-        <v>2.251043281062533e-237</v>
+        <v>1.968731119963541e-234</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5276401042938232</v>
+        <v>0.5784090161323547</v>
       </c>
       <c r="F42" t="n">
-        <v>62.37508771929825</v>
+        <v>35.10570945945949</v>
       </c>
       <c r="G42" t="n">
-        <v>0.1794285714285714</v>
+        <v>0.2525714285714286</v>
       </c>
       <c r="H42" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I42" t="n">
         <v>1</v>
@@ -3135,13 +3135,13 @@
         <v>0</v>
       </c>
       <c r="M42" t="n">
-        <v>3.64262843132019</v>
+        <v>4.464504241943359</v>
       </c>
       <c r="N42" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O42" t="n">
-        <v>9</v>
+        <v>12.9</v>
       </c>
       <c r="P42" t="n">
         <v>1</v>
@@ -3153,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="S42" t="n">
-        <v>3.642626047134399</v>
+        <v>4.46450138092041</v>
       </c>
       <c r="T42" t="n">
         <v>0</v>
@@ -3169,22 +3169,22 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.2229508147379738</v>
+        <v>0.1951219469495671</v>
       </c>
       <c r="D43" t="n">
-        <v>3.672046268824532e-155</v>
+        <v>2.380311982165284e-155</v>
       </c>
       <c r="E43" t="n">
-        <v>0.6513852477073669</v>
+        <v>0.6149226427078247</v>
       </c>
       <c r="F43" t="n">
-        <v>46.36296228391828</v>
+        <v>33.90739130434784</v>
       </c>
       <c r="G43" t="n">
-        <v>0.8869323447636701</v>
+        <v>0.4476367006487488</v>
       </c>
       <c r="H43" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I43" t="n">
         <v>1</v>
@@ -3199,13 +3199,13 @@
         <v>0</v>
       </c>
       <c r="M43" t="n">
-        <v>14.4165198802948</v>
+        <v>8.789872646331787</v>
       </c>
       <c r="N43" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O43" t="n">
-        <v>10.3</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="P43" t="n">
         <v>1</v>
@@ -3217,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="S43" t="n">
-        <v>14.41651749610901</v>
+        <v>8.789870023727417</v>
       </c>
       <c r="T43" t="n">
         <v>0</v>
@@ -3233,22 +3233,22 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.2139534848025961</v>
+        <v>0.2317596525189266</v>
       </c>
       <c r="D44" t="n">
-        <v>0.04548308581447544</v>
+        <v>7.197570537883027e-79</v>
       </c>
       <c r="E44" t="n">
-        <v>0.702419638633728</v>
+        <v>0.5893800854682922</v>
       </c>
       <c r="F44" t="n">
-        <v>19.06567472527476</v>
+        <v>31.66425393883227</v>
       </c>
       <c r="G44" t="n">
-        <v>0.3513203214695752</v>
+        <v>0.5568312284730195</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I44" t="n">
         <v>1</v>
@@ -3263,13 +3263,13 @@
         <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>8.233566284179688</v>
+        <v>8.946491718292236</v>
       </c>
       <c r="N44" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O44" t="n">
-        <v>11.1</v>
+        <v>10.9</v>
       </c>
       <c r="P44" t="n">
         <v>1</v>
@@ -3281,7 +3281,7 @@
         <v>0</v>
       </c>
       <c r="S44" t="n">
-        <v>8.233563899993896</v>
+        <v>8.946489572525024</v>
       </c>
       <c r="T44" t="n">
         <v>0</v>
@@ -3297,28 +3297,28 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.2531249968376953</v>
+        <v>0.1887417193182316</v>
       </c>
       <c r="D45" t="n">
-        <v>0.001161000163922509</v>
+        <v>1.382674377178161e-80</v>
       </c>
       <c r="E45" t="n">
-        <v>0.643058717250824</v>
+        <v>0.6188210248947144</v>
       </c>
       <c r="F45" t="n">
-        <v>43.61036492374728</v>
+        <v>18.30534883720932</v>
       </c>
       <c r="G45" t="n">
-        <v>0.2199067726898821</v>
+        <v>0.1853578283520702</v>
       </c>
       <c r="H45" t="n">
-        <v>0.875</v>
+        <v>0.625</v>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K45" t="n">
         <v>0.5</v>
@@ -3327,13 +3327,13 @@
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>8.612137079238892</v>
+        <v>16.5197057723999</v>
       </c>
       <c r="N45" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O45" t="n">
-        <v>11</v>
+        <v>11.2</v>
       </c>
       <c r="P45" t="n">
         <v>1</v>
@@ -3345,7 +3345,7 @@
         <v>0</v>
       </c>
       <c r="S45" t="n">
-        <v>8.612134218215942</v>
+        <v>16.51970386505127</v>
       </c>
       <c r="T45" t="n">
         <v>0</v>
@@ -3361,22 +3361,22 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.1860465090293132</v>
+        <v>0.2569343033344771</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0004175636360930292</v>
+        <v>0.004061682527016153</v>
       </c>
       <c r="E46" t="n">
-        <v>0.6352371573448181</v>
+        <v>0.6358121037483215</v>
       </c>
       <c r="F46" t="n">
-        <v>44.19500000000002</v>
+        <v>57.58092686002524</v>
       </c>
       <c r="G46" t="n">
-        <v>0.1758515646635281</v>
+        <v>0.225976183882581</v>
       </c>
       <c r="H46" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.5</v>
       </c>
       <c r="I46" t="n">
         <v>1</v>
@@ -3391,13 +3391,13 @@
         <v>0</v>
       </c>
       <c r="M46" t="n">
-        <v>7.088169574737549</v>
+        <v>7.788661956787109</v>
       </c>
       <c r="N46" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O46" t="n">
-        <v>9.4</v>
+        <v>8.9</v>
       </c>
       <c r="P46" t="n">
         <v>1</v>
@@ -3409,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="S46" t="n">
-        <v>7.088166952133179</v>
+        <v>7.788659811019897</v>
       </c>
       <c r="T46" t="n">
         <v>0</v>
@@ -3425,28 +3425,28 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.2504537162138465</v>
+        <v>0.3242187461542512</v>
       </c>
       <c r="D47" t="n">
-        <v>0.01213193248681383</v>
+        <v>0.009287435123470902</v>
       </c>
       <c r="E47" t="n">
-        <v>0.6774833202362061</v>
+        <v>0.6462003588676453</v>
       </c>
       <c r="F47" t="n">
-        <v>26.4068008658009</v>
+        <v>51.52598591549298</v>
       </c>
       <c r="G47" t="n">
-        <v>0.4914308489438023</v>
+        <v>0.3112793941809486</v>
       </c>
       <c r="H47" t="n">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="I47" t="n">
         <v>1</v>
       </c>
       <c r="J47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47" t="n">
         <v>0.5</v>
@@ -3455,13 +3455,13 @@
         <v>0</v>
       </c>
       <c r="M47" t="n">
-        <v>21.68769788742065</v>
+        <v>7.569626331329346</v>
       </c>
       <c r="N47" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O47" t="n">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
       <c r="P47" t="n">
         <v>1</v>
@@ -3473,7 +3473,7 @@
         <v>0</v>
       </c>
       <c r="S47" t="n">
-        <v>21.68769598007202</v>
+        <v>7.569623470306396</v>
       </c>
       <c r="T47" t="n">
         <v>0</v>
@@ -3489,22 +3489,22 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.308641970327694</v>
+        <v>0.2564102514135438</v>
       </c>
       <c r="D48" t="n">
-        <v>0.1022354989507534</v>
+        <v>0.08332543465763792</v>
       </c>
       <c r="E48" t="n">
-        <v>0.6561532616615295</v>
+        <v>0.64141845703125</v>
       </c>
       <c r="F48" t="n">
-        <v>64.04298982750998</v>
+        <v>54.46019230769235</v>
       </c>
       <c r="G48" t="n">
-        <v>1.06423982869379</v>
+        <v>0.987152034261242</v>
       </c>
       <c r="H48" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.5</v>
       </c>
       <c r="I48" t="n">
         <v>1</v>
@@ -3519,13 +3519,13 @@
         <v>0</v>
       </c>
       <c r="M48" t="n">
-        <v>7.537940979003906</v>
+        <v>5.44382643699646</v>
       </c>
       <c r="N48" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O48" t="n">
-        <v>11.3</v>
+        <v>9.1</v>
       </c>
       <c r="P48" t="n">
         <v>1</v>
@@ -3537,7 +3537,7 @@
         <v>0</v>
       </c>
       <c r="S48" t="n">
-        <v>7.537938356399536</v>
+        <v>5.44382381439209</v>
       </c>
       <c r="T48" t="n">
         <v>0</v>
@@ -3553,22 +3553,22 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.0434782600378072</v>
+        <v>0.1016949114622236</v>
       </c>
       <c r="D49" t="n">
-        <v>3.225165604459343e-237</v>
+        <v>4.770012214615472e-80</v>
       </c>
       <c r="E49" t="n">
-        <v>0.437296986579895</v>
+        <v>0.5940601825714111</v>
       </c>
       <c r="F49" t="n">
-        <v>3.344999999999999</v>
+        <v>33.58803571428575</v>
       </c>
       <c r="G49" t="n">
-        <v>0.1445086705202312</v>
+        <v>0.4739884393063584</v>
       </c>
       <c r="H49" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I49" t="n">
         <v>1</v>
@@ -3583,13 +3583,13 @@
         <v>0</v>
       </c>
       <c r="M49" t="n">
-        <v>6.361522912979126</v>
+        <v>7.083547592163086</v>
       </c>
       <c r="N49" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O49" t="n">
-        <v>9.6</v>
+        <v>11.5</v>
       </c>
       <c r="P49" t="n">
         <v>1</v>
@@ -3601,7 +3601,7 @@
         <v>0</v>
       </c>
       <c r="S49" t="n">
-        <v>6.361521005630493</v>
+        <v>7.083545446395874</v>
       </c>
       <c r="T49" t="n">
         <v>0</v>
@@ -3617,25 +3617,25 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.2456140300919942</v>
+        <v>0.2173912997269482</v>
       </c>
       <c r="D50" t="n">
-        <v>0.09492221173903496</v>
+        <v>0.02177394772860456</v>
       </c>
       <c r="E50" t="n">
-        <v>0.6636015772819519</v>
+        <v>0.6097381711006165</v>
       </c>
       <c r="F50" t="n">
-        <v>53.42040672268908</v>
+        <v>66.4384210526316</v>
       </c>
       <c r="G50" t="n">
-        <v>0.9406130268199234</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="H50" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.5</v>
       </c>
       <c r="I50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="n">
         <v>1</v>
@@ -3647,13 +3647,13 @@
         <v>0</v>
       </c>
       <c r="M50" t="n">
-        <v>5.903068542480469</v>
+        <v>5.050935506820679</v>
       </c>
       <c r="N50" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O50" t="n">
-        <v>11.5</v>
+        <v>9</v>
       </c>
       <c r="P50" t="n">
         <v>1</v>
@@ -3665,7 +3665,7 @@
         <v>0</v>
       </c>
       <c r="S50" t="n">
-        <v>5.903066873550415</v>
+        <v>5.050932884216309</v>
       </c>
       <c r="T50" t="n">
         <v>0</v>
@@ -3681,22 +3681,22 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.3402061809262408</v>
+        <v>0.2399999958230205</v>
       </c>
       <c r="D51" t="n">
-        <v>0.01924813803116057</v>
+        <v>0.02321946020470673</v>
       </c>
       <c r="E51" t="n">
-        <v>0.631574809551239</v>
+        <v>0.634426474571228</v>
       </c>
       <c r="F51" t="n">
-        <v>37.55622413793105</v>
+        <v>15.2357591324201</v>
       </c>
       <c r="G51" t="n">
-        <v>0.5326231691078562</v>
+        <v>0.474034620505992</v>
       </c>
       <c r="H51" t="n">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="I51" t="n">
         <v>1</v>
@@ -3711,13 +3711,13 @@
         <v>0</v>
       </c>
       <c r="M51" t="n">
-        <v>5.285675048828125</v>
+        <v>8.303726673126221</v>
       </c>
       <c r="N51" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O51" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P51" t="n">
         <v>1</v>
@@ -3729,7 +3729,7 @@
         <v>0</v>
       </c>
       <c r="S51" t="n">
-        <v>5.285672903060913</v>
+        <v>8.303724765777588</v>
       </c>
       <c r="T51" t="n">
         <v>0</v>
@@ -3745,28 +3745,28 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.1637010647828675</v>
+        <v>0.111940296236634</v>
       </c>
       <c r="D52" t="n">
-        <v>8.893036079598986e-81</v>
+        <v>5.174707510911508e-82</v>
       </c>
       <c r="E52" t="n">
-        <v>0.6043509244918823</v>
+        <v>0.5818077325820923</v>
       </c>
       <c r="F52" t="n">
-        <v>37.655008291874</v>
+        <v>37.9055614973262</v>
       </c>
       <c r="G52" t="n">
-        <v>0.2465554749818709</v>
+        <v>0.1907179115300943</v>
       </c>
       <c r="H52" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="I52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52" t="n">
         <v>0.5</v>
@@ -3775,13 +3775,13 @@
         <v>0</v>
       </c>
       <c r="M52" t="n">
-        <v>5.346846103668213</v>
+        <v>5.891186952590942</v>
       </c>
       <c r="N52" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O52" t="n">
-        <v>12.2</v>
+        <v>11.8</v>
       </c>
       <c r="P52" t="n">
         <v>1</v>
@@ -3793,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="S52" t="n">
-        <v>5.346843719482422</v>
+        <v>5.89118480682373</v>
       </c>
       <c r="T52" t="n">
         <v>0</v>
@@ -3809,19 +3809,19 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.3275434203040472</v>
+        <v>0.2835442999180901</v>
       </c>
       <c r="D53" t="n">
-        <v>0.01686448050214129</v>
+        <v>0.01798085043598062</v>
       </c>
       <c r="E53" t="n">
-        <v>0.6239048838615417</v>
+        <v>0.6190769672393799</v>
       </c>
       <c r="F53" t="n">
-        <v>38.98136752136756</v>
+        <v>55.3716666666667</v>
       </c>
       <c r="G53" t="n">
-        <v>0.3367129135538954</v>
+        <v>0.3489861259338314</v>
       </c>
       <c r="H53" t="n">
         <v>0.7142857142857143</v>
@@ -3839,13 +3839,13 @@
         <v>0</v>
       </c>
       <c r="M53" t="n">
-        <v>6.328605651855469</v>
+        <v>10.13561797142029</v>
       </c>
       <c r="N53" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O53" t="n">
-        <v>9</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="P53" t="n">
         <v>1</v>
@@ -3857,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="S53" t="n">
-        <v>6.328603267669678</v>
+        <v>10.1356155872345</v>
       </c>
       <c r="T53" t="n">
         <v>0</v>
@@ -3873,19 +3873,19 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.2784810081589489</v>
+        <v>0.2657807266268585</v>
       </c>
       <c r="D54" t="n">
-        <v>0.03760598806271453</v>
+        <v>0.03111386339672019</v>
       </c>
       <c r="E54" t="n">
-        <v>0.6445425152778625</v>
+        <v>0.6652542352676392</v>
       </c>
       <c r="F54" t="n">
-        <v>40.35087213740459</v>
+        <v>45.54193343386473</v>
       </c>
       <c r="G54" t="n">
-        <v>0.4944812362030905</v>
+        <v>0.4547461368653422</v>
       </c>
       <c r="H54" t="n">
         <v>0.1363636363636364</v>
@@ -3903,13 +3903,13 @@
         <v>0</v>
       </c>
       <c r="M54" t="n">
-        <v>9.471602916717529</v>
+        <v>9.067858457565308</v>
       </c>
       <c r="N54" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O54" t="n">
-        <v>10.9</v>
+        <v>10.8</v>
       </c>
       <c r="P54" t="n">
         <v>1</v>
@@ -3921,7 +3921,7 @@
         <v>0</v>
       </c>
       <c r="S54" t="n">
-        <v>9.47160005569458</v>
+        <v>9.067856073379517</v>
       </c>
       <c r="T54" t="n">
         <v>0</v>
@@ -3937,22 +3937,22 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.2977528045014834</v>
+        <v>0.1134751745271868</v>
       </c>
       <c r="D55" t="n">
-        <v>0.04857196635896474</v>
+        <v>8.837384123676883e-83</v>
       </c>
       <c r="E55" t="n">
-        <v>0.6339091062545776</v>
+        <v>0.5512097477912903</v>
       </c>
       <c r="F55" t="n">
-        <v>51.36293437264271</v>
+        <v>26.08375000000004</v>
       </c>
       <c r="G55" t="n">
-        <v>0.4799482535575679</v>
+        <v>0.2069857697283312</v>
       </c>
       <c r="H55" t="n">
-        <v>0.1052631578947368</v>
+        <v>0.05263157894736842</v>
       </c>
       <c r="I55" t="n">
         <v>1</v>
@@ -3967,13 +3967,13 @@
         <v>0</v>
       </c>
       <c r="M55" t="n">
-        <v>14.17187547683716</v>
+        <v>5.358141422271729</v>
       </c>
       <c r="N55" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O55" t="n">
-        <v>10.3</v>
+        <v>12.4</v>
       </c>
       <c r="P55" t="n">
         <v>1</v>
@@ -3985,7 +3985,7 @@
         <v>0</v>
       </c>
       <c r="S55" t="n">
-        <v>14.1718738079071</v>
+        <v>5.358139276504517</v>
       </c>
       <c r="T55" t="n">
         <v>0</v>
@@ -4001,22 +4001,22 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.114864862147553</v>
+        <v>0.08333333094135809</v>
       </c>
       <c r="D56" t="n">
-        <v>4.478462131344694e-159</v>
+        <v>6.711919286380671e-07</v>
       </c>
       <c r="E56" t="n">
-        <v>0.5457214713096619</v>
+        <v>0.5416167974472046</v>
       </c>
       <c r="F56" t="n">
-        <v>12.94901515151517</v>
+        <v>6.284166666666692</v>
       </c>
       <c r="G56" t="n">
-        <v>0.1971920867900447</v>
+        <v>0.175494575622208</v>
       </c>
       <c r="H56" t="n">
-        <v>0.04761904761904762</v>
+        <v>0</v>
       </c>
       <c r="I56" t="n">
         <v>1</v>
@@ -4031,13 +4031,13 @@
         <v>0</v>
       </c>
       <c r="M56" t="n">
-        <v>6.58995509147644</v>
+        <v>7.05184268951416</v>
       </c>
       <c r="N56" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O56" t="n">
-        <v>11.7</v>
+        <v>9.1</v>
       </c>
       <c r="P56" t="n">
         <v>1</v>
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="S56" t="n">
-        <v>6.589952945709229</v>
+        <v>7.051840543746948</v>
       </c>
       <c r="T56" t="n">
         <v>0</v>
@@ -4065,28 +4065,28 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.2481536144494458</v>
+        <v>0.160363081886657</v>
       </c>
       <c r="D57" t="n">
-        <v>0.01781453097330511</v>
+        <v>2.309659958056557e-79</v>
       </c>
       <c r="E57" t="n">
-        <v>0.5896622538566589</v>
+        <v>0.5953655242919922</v>
       </c>
       <c r="F57" t="n">
-        <v>41.55346821104195</v>
+        <v>37.20964285714288</v>
       </c>
       <c r="G57" t="n">
-        <v>0.481736733287388</v>
+        <v>0.4545141281874569</v>
       </c>
       <c r="H57" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I57" t="n">
         <v>1</v>
       </c>
       <c r="J57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K57" t="n">
         <v>0.5</v>
@@ -4095,13 +4095,13 @@
         <v>0</v>
       </c>
       <c r="M57" t="n">
-        <v>9.101379632949829</v>
+        <v>29.66759347915649</v>
       </c>
       <c r="N57" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O57" t="n">
-        <v>11</v>
+        <v>10.7</v>
       </c>
       <c r="P57" t="n">
         <v>1</v>
@@ -4113,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="S57" t="n">
-        <v>9.101377725601196</v>
+        <v>29.66759181022644</v>
       </c>
       <c r="T57" t="n">
         <v>0</v>
@@ -4129,28 +4129,28 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.2169811284215913</v>
+        <v>0.2982456098849646</v>
       </c>
       <c r="D58" t="n">
-        <v>8.876118552529123e-157</v>
+        <v>5.587374823377171e-156</v>
       </c>
       <c r="E58" t="n">
-        <v>0.6197860836982727</v>
+        <v>0.6677335500717163</v>
       </c>
       <c r="F58" t="n">
-        <v>36.59133064516129</v>
+        <v>55.80548986486485</v>
       </c>
       <c r="G58" t="n">
-        <v>0.3542116630669546</v>
+        <v>0.4384449244060475</v>
       </c>
       <c r="H58" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I58" t="n">
         <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58" t="n">
         <v>0.5</v>
@@ -4159,13 +4159,13 @@
         <v>0</v>
       </c>
       <c r="M58" t="n">
-        <v>4.845703840255737</v>
+        <v>4.787078380584717</v>
       </c>
       <c r="N58" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O58" t="n">
-        <v>9</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="P58" t="n">
         <v>1</v>
@@ -4177,7 +4177,7 @@
         <v>0</v>
       </c>
       <c r="S58" t="n">
-        <v>4.845701932907104</v>
+        <v>4.787076950073242</v>
       </c>
       <c r="T58" t="n">
         <v>0</v>
@@ -4193,25 +4193,25 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.2428571378938776</v>
+        <v>0.2542372831715025</v>
       </c>
       <c r="D59" t="n">
-        <v>8.911790229777884e-79</v>
+        <v>3.589538320049e-155</v>
       </c>
       <c r="E59" t="n">
-        <v>0.622794508934021</v>
+        <v>0.6443840861320496</v>
       </c>
       <c r="F59" t="n">
-        <v>31.1552923387097</v>
+        <v>42.37415205261064</v>
       </c>
       <c r="G59" t="n">
-        <v>1.170454545454545</v>
+        <v>0.8459595959595959</v>
       </c>
       <c r="H59" t="n">
         <v>1</v>
       </c>
       <c r="I59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J59" t="n">
         <v>1</v>
@@ -4223,13 +4223,13 @@
         <v>0</v>
       </c>
       <c r="M59" t="n">
-        <v>9.041645765304565</v>
+        <v>7.540828943252563</v>
       </c>
       <c r="N59" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O59" t="n">
-        <v>10.9</v>
+        <v>11.3</v>
       </c>
       <c r="P59" t="n">
         <v>1</v>
@@ -4241,7 +4241,7 @@
         <v>0</v>
       </c>
       <c r="S59" t="n">
-        <v>9.041643619537354</v>
+        <v>7.540826559066772</v>
       </c>
       <c r="T59" t="n">
         <v>0</v>
@@ -4257,28 +4257,28 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.2085661051193436</v>
+        <v>0.2117202241202683</v>
       </c>
       <c r="D60" t="n">
-        <v>0.001358219974730529</v>
+        <v>0.0003559680387984924</v>
       </c>
       <c r="E60" t="n">
-        <v>0.6309710144996643</v>
+        <v>0.6252592802047729</v>
       </c>
       <c r="F60" t="n">
-        <v>39.51730563314715</v>
+        <v>28.42193719593101</v>
       </c>
       <c r="G60" t="n">
-        <v>0.2127882599580713</v>
+        <v>0.1858839972047519</v>
       </c>
       <c r="H60" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I60" t="n">
         <v>1</v>
       </c>
       <c r="J60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" t="n">
         <v>0.5</v>
@@ -4287,13 +4287,13 @@
         <v>0</v>
       </c>
       <c r="M60" t="n">
-        <v>6.550629138946533</v>
+        <v>7.067922592163086</v>
       </c>
       <c r="N60" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O60" t="n">
-        <v>9.4</v>
+        <v>9.1</v>
       </c>
       <c r="P60" t="n">
         <v>1</v>
@@ -4305,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="S60" t="n">
-        <v>6.550626277923584</v>
+        <v>7.067920684814453</v>
       </c>
       <c r="T60" t="n">
         <v>0</v>
@@ -4321,19 +4321,19 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.08571428242959198</v>
+        <v>0.1764705848799741</v>
       </c>
       <c r="D61" t="n">
-        <v>8.439601420831656e-232</v>
+        <v>3.138531287068738e-155</v>
       </c>
       <c r="E61" t="n">
-        <v>0.5335611701011658</v>
+        <v>0.5446386337280273</v>
       </c>
       <c r="F61" t="n">
-        <v>25.10457036114573</v>
+        <v>32.92352941176475</v>
       </c>
       <c r="G61" t="n">
-        <v>2.477732793522267</v>
+        <v>2.37246963562753</v>
       </c>
       <c r="H61" t="n">
         <v>1</v>
@@ -4351,13 +4351,13 @@
         <v>0</v>
       </c>
       <c r="M61" t="n">
-        <v>6.037535905838013</v>
+        <v>5.945929765701294</v>
       </c>
       <c r="N61" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O61" t="n">
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="P61" t="n">
         <v>1</v>
@@ -4369,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="S61" t="n">
-        <v>6.037533760070801</v>
+        <v>5.945927619934082</v>
       </c>
       <c r="T61" t="n">
         <v>0</v>
@@ -4385,19 +4385,19 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.2937062887084944</v>
+        <v>0.1587301538561352</v>
       </c>
       <c r="D62" t="n">
-        <v>3.530298853742955e-155</v>
+        <v>1.950202647751698e-155</v>
       </c>
       <c r="E62" t="n">
-        <v>0.6853580474853516</v>
+        <v>0.5793384313583374</v>
       </c>
       <c r="F62" t="n">
-        <v>52.56600000000003</v>
+        <v>33.39307218309861</v>
       </c>
       <c r="G62" t="n">
-        <v>1.035</v>
+        <v>0.8825</v>
       </c>
       <c r="H62" t="n">
         <v>1</v>
@@ -4415,13 +4415,13 @@
         <v>0</v>
       </c>
       <c r="M62" t="n">
-        <v>5.432528495788574</v>
+        <v>4.710731506347656</v>
       </c>
       <c r="N62" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O62" t="n">
-        <v>9.199999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="P62" t="n">
         <v>1</v>
@@ -4433,7 +4433,7 @@
         <v>0</v>
       </c>
       <c r="S62" t="n">
-        <v>5.432526350021362</v>
+        <v>4.710729598999023</v>
       </c>
       <c r="T62" t="n">
         <v>0</v>
@@ -4449,19 +4449,19 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.1893491090732118</v>
+        <v>0.2254901915402731</v>
       </c>
       <c r="D63" t="n">
-        <v>2.155190947883263e-80</v>
+        <v>1.831608585351408e-155</v>
       </c>
       <c r="E63" t="n">
-        <v>0.6318918466567993</v>
+        <v>0.6494846940040588</v>
       </c>
       <c r="F63" t="n">
-        <v>40.29500000000002</v>
+        <v>47.82300000000004</v>
       </c>
       <c r="G63" t="n">
-        <v>0.3347280334728033</v>
+        <v>0.6373779637377964</v>
       </c>
       <c r="H63" t="n">
         <v>0.5</v>
@@ -4479,13 +4479,13 @@
         <v>0</v>
       </c>
       <c r="M63" t="n">
-        <v>5.217766284942627</v>
+        <v>4.407897233963013</v>
       </c>
       <c r="N63" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O63" t="n">
-        <v>12.5</v>
+        <v>13.2</v>
       </c>
       <c r="P63" t="n">
         <v>1</v>
@@ -4497,7 +4497,7 @@
         <v>0</v>
       </c>
       <c r="S63" t="n">
-        <v>5.217764616012573</v>
+        <v>4.407895088195801</v>
       </c>
       <c r="T63" t="n">
         <v>0</v>
@@ -4513,22 +4513,22 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.2127659540163976</v>
+        <v>0.2711864359730601</v>
       </c>
       <c r="D64" t="n">
-        <v>1.984846057827382e-156</v>
+        <v>1.95311839983281e-155</v>
       </c>
       <c r="E64" t="n">
-        <v>0.6314188838005066</v>
+        <v>0.6503112316131592</v>
       </c>
       <c r="F64" t="n">
-        <v>44.16500000000002</v>
+        <v>51.77572727272729</v>
       </c>
       <c r="G64" t="n">
-        <v>0.380327868852459</v>
+        <v>0.6540983606557377</v>
       </c>
       <c r="H64" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I64" t="n">
         <v>1</v>
@@ -4543,10 +4543,10 @@
         <v>0</v>
       </c>
       <c r="M64" t="n">
-        <v>4.644629955291748</v>
+        <v>4.68550443649292</v>
       </c>
       <c r="N64" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O64" t="n">
         <v>9</v>
@@ -4561,7 +4561,7 @@
         <v>0</v>
       </c>
       <c r="S64" t="n">
-        <v>4.644628047943115</v>
+        <v>4.685502290725708</v>
       </c>
       <c r="T64" t="n">
         <v>0</v>
@@ -4577,19 +4577,19 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.3105590013517998</v>
+        <v>0.1718749960986329</v>
       </c>
       <c r="D65" t="n">
-        <v>8.605951974046729e-79</v>
+        <v>3.700535364930801e-156</v>
       </c>
       <c r="E65" t="n">
-        <v>0.6449974775314331</v>
+        <v>0.6151825189590454</v>
       </c>
       <c r="F65" t="n">
-        <v>72.27625000000003</v>
+        <v>50.06250000000003</v>
       </c>
       <c r="G65" t="n">
-        <v>0.7555110220440882</v>
+        <v>0.5350701402805611</v>
       </c>
       <c r="H65" t="n">
         <v>1</v>
@@ -4607,13 +4607,13 @@
         <v>0</v>
       </c>
       <c r="M65" t="n">
-        <v>4.426775932312012</v>
+        <v>7.968134641647339</v>
       </c>
       <c r="N65" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O65" t="n">
-        <v>13.1</v>
+        <v>11.2</v>
       </c>
       <c r="P65" t="n">
         <v>1</v>
@@ -4625,7 +4625,7 @@
         <v>0</v>
       </c>
       <c r="S65" t="n">
-        <v>4.426774501800537</v>
+        <v>7.968132734298706</v>
       </c>
       <c r="T65" t="n">
         <v>0</v>
@@ -4641,28 +4641,28 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>0.1290322548132733</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>8.343066498983699e-156</v>
       </c>
       <c r="E66" t="n">
-        <v>0.1999654471874237</v>
+        <v>0.6512388586997986</v>
       </c>
       <c r="F66" t="n">
-        <v>0</v>
+        <v>1.684090909090912</v>
       </c>
       <c r="G66" t="n">
-        <v>0.05269761606022585</v>
+        <v>0.3851944792973651</v>
       </c>
       <c r="H66" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="I66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K66" t="n">
         <v>0.5</v>
@@ -4671,13 +4671,13 @@
         <v>0</v>
       </c>
       <c r="M66" t="n">
-        <v>10.66058039665222</v>
+        <v>10.87006783485413</v>
       </c>
       <c r="N66" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O66" t="n">
-        <v>10.1</v>
+        <v>10.7</v>
       </c>
       <c r="P66" t="n">
         <v>1</v>
@@ -4689,7 +4689,7 @@
         <v>0</v>
       </c>
       <c r="S66" t="n">
-        <v>10.66057920455933</v>
+        <v>10.87006592750549</v>
       </c>
       <c r="T66" t="n">
         <v>0</v>
@@ -4705,28 +4705,28 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.3098591501333511</v>
+        <v>0.2080924817000234</v>
       </c>
       <c r="D67" t="n">
-        <v>3.25712006452215e-155</v>
+        <v>3.196581908133926e-156</v>
       </c>
       <c r="E67" t="n">
-        <v>0.6250879764556885</v>
+        <v>0.5914371609687805</v>
       </c>
       <c r="F67" t="n">
-        <v>58.80052830188683</v>
+        <v>39.06056818181818</v>
       </c>
       <c r="G67" t="n">
-        <v>0.6808219178082192</v>
+        <v>0.3726027397260274</v>
       </c>
       <c r="H67" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="I67" t="n">
         <v>1</v>
       </c>
       <c r="J67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K67" t="n">
         <v>0.5</v>
@@ -4735,13 +4735,13 @@
         <v>0</v>
       </c>
       <c r="M67" t="n">
-        <v>7.306503295898438</v>
+        <v>5.990576982498169</v>
       </c>
       <c r="N67" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O67" t="n">
-        <v>10.1</v>
+        <v>9.1</v>
       </c>
       <c r="P67" t="n">
         <v>1</v>
@@ -4753,7 +4753,7 @@
         <v>0</v>
       </c>
       <c r="S67" t="n">
-        <v>7.306501626968384</v>
+        <v>5.990574836730957</v>
       </c>
       <c r="T67" t="n">
         <v>0</v>
@@ -4769,19 +4769,19 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.06611570131650846</v>
+        <v>0.1594202879174543</v>
       </c>
       <c r="D68" t="n">
-        <v>1.124448887274863e-155</v>
+        <v>1.799020134544166e-155</v>
       </c>
       <c r="E68" t="n">
-        <v>0.4563247263431549</v>
+        <v>0.4732628762722015</v>
       </c>
       <c r="F68" t="n">
-        <v>32.81282117163414</v>
+        <v>37.72273060700533</v>
       </c>
       <c r="G68" t="n">
-        <v>12.28346456692913</v>
+        <v>6.78740157480315</v>
       </c>
       <c r="H68" t="n">
         <v>1</v>
@@ -4790,7 +4790,7 @@
         <v>1</v>
       </c>
       <c r="J68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K68" t="n">
         <v>0.5</v>
@@ -4799,13 +4799,13 @@
         <v>0</v>
       </c>
       <c r="M68" t="n">
-        <v>19.78692579269409</v>
+        <v>11.80241847038269</v>
       </c>
       <c r="N68" t="n">
-        <v>2079.56640625</v>
+        <v>2153.53125</v>
       </c>
       <c r="O68" t="n">
-        <v>10.8</v>
+        <v>10.5</v>
       </c>
       <c r="P68" t="n">
         <v>1</v>
@@ -4817,7 +4817,7 @@
         <v>0</v>
       </c>
       <c r="S68" t="n">
-        <v>19.7869234085083</v>
+        <v>11.8024160861969</v>
       </c>
       <c r="T68" t="n">
         <v>0</v>

</xml_diff>